<commit_message>
Fix unit tests and support PLACE_TYPE
</commit_message>
<xml_diff>
--- a/test/data/convert-contact-forms/forms/contact/district_hospital.xlsx
+++ b/test/data/convert-contact-forms/forms/contact/district_hospital.xlsx
@@ -1,194 +1,196 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="choices" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="settings" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="survey" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="choices" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="settings" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>relevant</t>
-  </si>
-  <si>
-    <t>appearance</t>
-  </si>
-  <si>
-    <t>constraint</t>
-  </si>
-  <si>
-    <t>constraint_message</t>
-  </si>
-  <si>
-    <t>calculation</t>
-  </si>
-  <si>
-    <t>choice_filter</t>
-  </si>
-  <si>
-    <t>hint</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>begin group</t>
-  </si>
-  <si>
-    <t>inputs</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>facility_id</t>
-  </si>
-  <si>
-    <t>Facility ID for the parent user</t>
-  </si>
-  <si>
-    <t>end group</t>
-  </si>
-  <si>
-    <t>contact</t>
-  </si>
-  <si>
-    <t>Branch Information</t>
-  </si>
-  <si>
-    <t>field-list</t>
-  </si>
-  <si>
-    <t>district_name</t>
-  </si>
-  <si>
-    <t>Branch Name</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Primary Contact</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>debug_note</t>
-  </si>
-  <si>
-    <t>DEBUG
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relevant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">appearance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constraint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constraint_message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choice_filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">begin group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facility ID for the parent user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">field-list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">district_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary Contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debug_note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEBUG
 User's facility ID: ${facility_id}</t>
   </si>
   <si>
-    <t>Names</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>contact_notes</t>
-  </si>
-  <si>
-    <t>Contact Notes</t>
-  </si>
-  <si>
-    <t>district_hospital</t>
-  </si>
-  <si>
-    <t>mandatory</t>
-  </si>
-  <si>
-    <t>calculate</t>
-  </si>
-  <si>
-    <t>${district_name}</t>
-  </si>
-  <si>
-    <t>list_name</t>
-  </si>
-  <si>
-    <t>yes_no</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>male_female</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>boy_girl</t>
-  </si>
-  <si>
-    <t>Girl</t>
-  </si>
-  <si>
-    <t>form_title</t>
-  </si>
-  <si>
-    <t>form_id</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>style</t>
-  </si>
-  <si>
-    <t>New District</t>
-  </si>
-  <si>
-    <t>district</t>
-  </si>
-  <si>
-    <t>2016-04-25</t>
+    <t xml:space="preserve">Names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact_notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">district_hospital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mandatory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${district_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male_female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boy_girl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Girl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">style</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New District</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-04-25</t>
   </si>
 </sst>
 </file>
@@ -196,9 +198,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -298,24 +300,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -323,47 +321,37 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Note" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -438,116 +426,203 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z65536"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.8112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.70918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.0867346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.22448979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="52.6377551020408"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.0867346938776"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.4030612244898"/>
-    <col collapsed="false" hidden="false" max="26" min="13" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="16.2908163265306"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="68.81"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="52.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="13" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="1" width="16.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" s="4" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" s="3" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
       <c r="E3" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" s="4" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" s="3" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -557,31 +632,11 @@
       <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" s="4" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" s="3" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
@@ -626,11 +681,11 @@
       <c r="L7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -640,32 +695,22 @@
       <c r="J8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -673,22 +718,22 @@
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="7" t="n">
+      <c r="E11" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -735,13 +780,13 @@
       <c r="L13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F14" s="3"/>
@@ -759,29 +804,20 @@
         <v>33</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="K15" s="0" t="s">
+      <c r="K15" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+    <row r="16" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
@@ -1821,34 +1857,14 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:A2,A17:A1048555,A6:A7,A9:A10,A15:A16,A12:A13">
+  <conditionalFormatting sqref="A3:A5 A8 A11 A14">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A5">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>"begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>"begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>"begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>"begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1857,88 +1873,88 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C65536"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.6071428571429"/>
-    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="8.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="16.2908163265306"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="83.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="1" width="8.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="1" width="16.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1952,8 +1968,8 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1962,73 +1978,73 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.4285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4897959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.6989795918367"/>
-    <col collapsed="false" hidden="false" max="26" min="7" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="16.2908163265306"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="36.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="1" width="16.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -2036,8 +2052,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
feat(#537)!: error when form internalId does not match file name (#776)
</commit_message>
<xml_diff>
--- a/test/data/convert-contact-forms/forms/contact/district_hospital.xlsx
+++ b/test/data/convert-contact-forms/forms/contact/district_hospital.xlsx
@@ -1,194 +1,196 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="choices" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="settings" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="survey" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="choices" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="settings" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>relevant</t>
-  </si>
-  <si>
-    <t>appearance</t>
-  </si>
-  <si>
-    <t>constraint</t>
-  </si>
-  <si>
-    <t>constraint_message</t>
-  </si>
-  <si>
-    <t>calculation</t>
-  </si>
-  <si>
-    <t>choice_filter</t>
-  </si>
-  <si>
-    <t>hint</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>begin group</t>
-  </si>
-  <si>
-    <t>inputs</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>facility_id</t>
-  </si>
-  <si>
-    <t>Facility ID for the parent user</t>
-  </si>
-  <si>
-    <t>end group</t>
-  </si>
-  <si>
-    <t>contact</t>
-  </si>
-  <si>
-    <t>Branch Information</t>
-  </si>
-  <si>
-    <t>field-list</t>
-  </si>
-  <si>
-    <t>district_name</t>
-  </si>
-  <si>
-    <t>Branch Name</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Primary Contact</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>debug_note</t>
-  </si>
-  <si>
-    <t>DEBUG
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relevant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">appearance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constraint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constraint_message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choice_filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">begin group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facility ID for the parent user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">field-list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">district_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary Contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debug_note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEBUG
 User's facility ID: ${facility_id}</t>
   </si>
   <si>
-    <t>Names</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>contact_notes</t>
-  </si>
-  <si>
-    <t>Contact Notes</t>
-  </si>
-  <si>
-    <t>district_hospital</t>
-  </si>
-  <si>
-    <t>mandatory</t>
-  </si>
-  <si>
-    <t>calculate</t>
-  </si>
-  <si>
-    <t>${district_name}</t>
-  </si>
-  <si>
-    <t>list_name</t>
-  </si>
-  <si>
-    <t>yes_no</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>male_female</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>boy_girl</t>
-  </si>
-  <si>
-    <t>Girl</t>
-  </si>
-  <si>
-    <t>form_title</t>
-  </si>
-  <si>
-    <t>form_id</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>style</t>
-  </si>
-  <si>
-    <t>New District</t>
-  </si>
-  <si>
-    <t>district</t>
-  </si>
-  <si>
-    <t>2016-04-25</t>
+    <t xml:space="preserve">Names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact_notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">district_hospital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mandatory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${district_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male_female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boy_girl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Girl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">form_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">style</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New District</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-04-25</t>
   </si>
 </sst>
 </file>
@@ -196,9 +198,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -298,24 +300,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -323,47 +321,37 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Note" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -438,116 +426,203 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z65536"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.8112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.70918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.0867346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.22448979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="52.6377551020408"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.0867346938776"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.4030612244898"/>
-    <col collapsed="false" hidden="false" max="26" min="13" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="16.2908163265306"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="68.81"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="52.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="13" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="1" width="16.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" s="4" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" s="3" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
       <c r="E3" s="3" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" s="4" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" s="3" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -557,31 +632,11 @@
       <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" s="4" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" s="3" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
@@ -626,11 +681,11 @@
       <c r="L7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -640,32 +695,22 @@
       <c r="J8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -673,22 +718,22 @@
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="7" t="n">
+      <c r="E11" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -735,13 +780,13 @@
       <c r="L13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F14" s="3"/>
@@ -759,29 +804,20 @@
         <v>33</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="K15" s="0" t="s">
+      <c r="K15" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+    <row r="16" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
@@ -1821,34 +1857,14 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:A2,A17:A1048555,A6:A7,A9:A10,A15:A16,A12:A13">
+  <conditionalFormatting sqref="A3:A5 A8 A11 A14">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:A5">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>"begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8">
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>"begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>"begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>"begin group"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1857,88 +1873,88 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C65536"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="83.6071428571429"/>
-    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="8.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="16.2908163265306"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="83.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="1" width="8.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="1" width="16.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1952,8 +1968,8 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1962,73 +1978,73 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.4285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4897959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.6989795918367"/>
-    <col collapsed="false" hidden="false" max="26" min="7" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="16.2908163265306"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="36.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="1" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="1" width="16.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -2036,8 +2052,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>